<commit_message>
criação do arquivo em pdf para ser acessível sem excel.
</commit_message>
<xml_diff>
--- a/Daily Schedule Excel Template-PT.xlsx
+++ b/Daily Schedule Excel Template-PT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Comercial\Desktop\cronograma de estudo mateus\planilha-agenda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mateus\agenda\planilha-agenda\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EFE1A2-977A-427C-B151-4B543D194E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9975" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -122,7 +123,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
@@ -519,7 +520,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -546,26 +547,25 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -580,7 +580,7 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -825,14 +825,20 @@
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>214630</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>337095</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>482599</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -865,14 +871,14 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="1">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -882,7 +888,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -912,7 +918,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -945,14 +957,14 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="1">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -962,7 +974,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -985,14 +997,20 @@
       <xdr:rowOff>65314</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1626465</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1245465</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>32657</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagem 3"/>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1025,17 +1043,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:H32" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="A3:H32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:H32" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="A3:H32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Column1" dataDxfId="7"/>
-    <tableColumn id="2" name="Column2" dataDxfId="6"/>
-    <tableColumn id="3" name="Column3" dataDxfId="5"/>
-    <tableColumn id="4" name="Column4" dataDxfId="4"/>
-    <tableColumn id="5" name="Column5" dataDxfId="3"/>
-    <tableColumn id="6" name="Column6" dataDxfId="2"/>
-    <tableColumn id="7" name="Column7" dataDxfId="1"/>
-    <tableColumn id="8" name="Column8" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1362,29 +1380,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:BP209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H32" sqref="A1:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="2" width="11.5" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:68" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1517,19 +1540,19 @@
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="24" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="7" t="s">
@@ -1597,16 +1620,16 @@
       <c r="BP3" s="2"/>
     </row>
     <row r="4" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="21">
+      <c r="A4" s="20">
         <v>0.29166666666666669</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="24"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="23"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -1669,16 +1692,16 @@
       <c r="BP4" s="2"/>
     </row>
     <row r="5" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
+      <c r="A5" s="21">
         <v>0.3125</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="24"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="23"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -1741,16 +1764,16 @@
       <c r="BP5" s="2"/>
     </row>
     <row r="6" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21">
+      <c r="A6" s="20">
         <v>0.33333333333333331</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="24"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="23"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -1813,16 +1836,16 @@
       <c r="BP6" s="2"/>
     </row>
     <row r="7" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22">
+      <c r="A7" s="21">
         <v>0.35416666666666702</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="24"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="23"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -1885,16 +1908,16 @@
       <c r="BP7" s="2"/>
     </row>
     <row r="8" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
+      <c r="A8" s="20">
         <v>0.375</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="24"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="23"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -1957,18 +1980,18 @@
       <c r="BP8" s="2"/>
     </row>
     <row r="9" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A9" s="22">
+      <c r="A9" s="21">
         <v>0.39583333333333398</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28" t="s">
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="24"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="23"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -2031,16 +2054,16 @@
       <c r="BP9" s="2"/>
     </row>
     <row r="10" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
+      <c r="A10" s="20">
         <v>0.41666666666666702</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="24"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="23"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -2103,16 +2126,16 @@
       <c r="BP10" s="2"/>
     </row>
     <row r="11" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+      <c r="A11" s="21">
         <v>0.4375</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="24"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="23"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -2175,16 +2198,16 @@
       <c r="BP11" s="2"/>
     </row>
     <row r="12" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
+      <c r="A12" s="20">
         <v>0.45833333333333398</v>
       </c>
       <c r="B12" s="5"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="24"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="23"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -2247,16 +2270,16 @@
       <c r="BP12" s="2"/>
     </row>
     <row r="13" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22">
+      <c r="A13" s="21">
         <v>0.47916666666666702</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="24"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="23"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -2319,18 +2342,18 @@
       <c r="BP13" s="2"/>
     </row>
     <row r="14" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21">
+      <c r="A14" s="20">
         <v>0.5</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="29" t="s">
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="24"/>
+      <c r="H14" s="23"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -2393,15 +2416,15 @@
       <c r="BP14" s="2"/>
     </row>
     <row r="15" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
+      <c r="A15" s="21">
         <v>0.52083333333333304</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="29" t="s">
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="28" t="s">
         <v>24</v>
       </c>
       <c r="H15" s="5"/>
@@ -2467,19 +2490,19 @@
       <c r="BP15" s="2"/>
     </row>
     <row r="16" spans="1:68" ht="36" x14ac:dyDescent="0.25">
-      <c r="A16" s="21">
+      <c r="A16" s="20">
         <v>0.54166666666666696</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="29" t="s">
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="G16" s="28" t="s">
         <v>24</v>
       </c>
       <c r="H16" s="5"/>
@@ -2545,23 +2568,23 @@
       <c r="BP16" s="2"/>
     </row>
     <row r="17" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22">
+      <c r="A17" s="21">
         <v>0.5625</v>
       </c>
       <c r="B17" s="5"/>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="30" t="s">
         <v>25</v>
       </c>
       <c r="H17" s="5"/>
@@ -2627,23 +2650,23 @@
       <c r="BP17" s="2"/>
     </row>
     <row r="18" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
+      <c r="A18" s="20">
         <v>0.58333333333333304</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="31" t="s">
+      <c r="G18" s="30" t="s">
         <v>25</v>
       </c>
       <c r="H18" s="5"/>
@@ -2709,23 +2732,23 @@
       <c r="BP18" s="2"/>
     </row>
     <row r="19" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22">
+      <c r="A19" s="21">
         <v>0.60416666666666696</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="31" t="s">
+      <c r="G19" s="30" t="s">
         <v>25</v>
       </c>
       <c r="H19" s="5"/>
@@ -2791,23 +2814,23 @@
       <c r="BP19" s="2"/>
     </row>
     <row r="20" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21">
+      <c r="A20" s="20">
         <v>0.625</v>
       </c>
       <c r="B20" s="1"/>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="30" t="s">
         <v>25</v>
       </c>
       <c r="H20" s="5"/>
@@ -2873,23 +2896,23 @@
       <c r="BP20" s="2"/>
     </row>
     <row r="21" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22">
+      <c r="A21" s="21">
         <v>0.64583333333333304</v>
       </c>
       <c r="B21" s="1"/>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="31" t="s">
+      <c r="G21" s="30" t="s">
         <v>26</v>
       </c>
       <c r="H21" s="5"/>
@@ -2955,23 +2978,23 @@
       <c r="BP21" s="2"/>
     </row>
     <row r="22" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21">
+      <c r="A22" s="20">
         <v>0.66666666666666696</v>
       </c>
       <c r="B22" s="1"/>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="31" t="s">
+      <c r="F22" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="G22" s="31" t="s">
+      <c r="G22" s="30" t="s">
         <v>26</v>
       </c>
       <c r="H22" s="5"/>
@@ -3037,23 +3060,23 @@
       <c r="BP22" s="2"/>
     </row>
     <row r="23" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22">
+      <c r="A23" s="21">
         <v>0.6875</v>
       </c>
       <c r="B23" s="1"/>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="31" t="s">
+      <c r="F23" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="G23" s="31" t="s">
+      <c r="G23" s="30" t="s">
         <v>26</v>
       </c>
       <c r="H23" s="5"/>
@@ -3119,23 +3142,23 @@
       <c r="BP23" s="2"/>
     </row>
     <row r="24" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21">
+      <c r="A24" s="20">
         <v>0.70833333333333304</v>
       </c>
       <c r="B24" s="1"/>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="31" t="s">
+      <c r="F24" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="G24" s="31" t="s">
+      <c r="G24" s="30" t="s">
         <v>26</v>
       </c>
       <c r="H24" s="5"/>
@@ -3201,23 +3224,23 @@
       <c r="BP24" s="2"/>
     </row>
     <row r="25" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22">
+      <c r="A25" s="21">
         <v>0.72916666666666696</v>
       </c>
       <c r="B25" s="1"/>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="31" t="s">
+      <c r="F25" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="G25" s="29" t="s">
+      <c r="G25" s="28" t="s">
         <v>30</v>
       </c>
       <c r="H25" s="5"/>
@@ -3283,23 +3306,23 @@
       <c r="BP25" s="2"/>
     </row>
     <row r="26" spans="1:68" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21">
+      <c r="A26" s="20">
         <v>0.75</v>
       </c>
       <c r="B26" s="1"/>
-      <c r="C26" s="31" t="s">
+      <c r="C26" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="31" t="s">
+      <c r="E26" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="31" t="s">
+      <c r="F26" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="G26" s="29" t="s">
+      <c r="G26" s="28" t="s">
         <v>30</v>
       </c>
       <c r="H26" s="5"/>
@@ -3365,23 +3388,23 @@
       <c r="BP26" s="2"/>
     </row>
     <row r="27" spans="1:68" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22">
+      <c r="A27" s="21">
         <v>0.77083333333333304</v>
       </c>
       <c r="B27" s="1"/>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="31" t="s">
+      <c r="E27" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="29" t="s">
+      <c r="F27" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G27" s="29" t="s">
+      <c r="G27" s="28" t="s">
         <v>29</v>
       </c>
       <c r="H27" s="5"/>
@@ -3447,23 +3470,23 @@
       <c r="BP27" s="2"/>
     </row>
     <row r="28" spans="1:68" ht="36" x14ac:dyDescent="0.25">
-      <c r="A28" s="21">
+      <c r="A28" s="20">
         <v>0.79166666666666696</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="29" t="s">
+      <c r="D28" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E28" s="29" t="s">
+      <c r="E28" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="F28" s="29" t="s">
+      <c r="F28" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G28" s="29" t="s">
+      <c r="G28" s="28" t="s">
         <v>29</v>
       </c>
       <c r="H28" s="5"/>
@@ -3529,23 +3552,23 @@
       <c r="BP28" s="2"/>
     </row>
     <row r="29" spans="1:68" ht="36" x14ac:dyDescent="0.25">
-      <c r="A29" s="22">
+      <c r="A29" s="21">
         <v>0.8125</v>
       </c>
       <c r="B29" s="1"/>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="29" t="s">
+      <c r="E29" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="F29" s="29" t="s">
+      <c r="F29" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G29" s="29" t="s">
+      <c r="G29" s="28" t="s">
         <v>29</v>
       </c>
       <c r="H29" s="5"/>
@@ -3611,23 +3634,23 @@
       <c r="BP29" s="2"/>
     </row>
     <row r="30" spans="1:68" ht="36" x14ac:dyDescent="0.25">
-      <c r="A30" s="21">
+      <c r="A30" s="20">
         <v>0.83333333333333304</v>
       </c>
       <c r="B30" s="1"/>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="29" t="s">
+      <c r="D30" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E30" s="29" t="s">
+      <c r="E30" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="29" t="s">
+      <c r="F30" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G30" s="29" t="s">
+      <c r="G30" s="28" t="s">
         <v>29</v>
       </c>
       <c r="H30" s="5"/>
@@ -3693,23 +3716,23 @@
       <c r="BP30" s="2"/>
     </row>
     <row r="31" spans="1:68" ht="36" x14ac:dyDescent="0.25">
-      <c r="A31" s="22">
+      <c r="A31" s="21">
         <v>0.85416666666666696</v>
       </c>
       <c r="B31" s="1"/>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="29" t="s">
+      <c r="D31" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="29" t="s">
+      <c r="E31" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="F31" s="29" t="s">
+      <c r="F31" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G31" s="29" t="s">
+      <c r="G31" s="28" t="s">
         <v>29</v>
       </c>
       <c r="H31" s="5"/>
@@ -3775,23 +3798,23 @@
       <c r="BP31" s="2"/>
     </row>
     <row r="32" spans="1:68" ht="36" x14ac:dyDescent="0.25">
-      <c r="A32" s="23">
+      <c r="A32" s="22">
         <v>0.875</v>
       </c>
       <c r="B32" s="8"/>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E32" s="29" t="s">
+      <c r="E32" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="F32" s="29" t="s">
+      <c r="F32" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G32" s="29" t="s">
+      <c r="G32" s="28" t="s">
         <v>29</v>
       </c>
       <c r="H32" s="9"/>
@@ -3999,12 +4022,12 @@
     <row r="35" spans="1:68" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
       <c r="B35" s="17"/>
-      <c r="C35" s="39" t="s">
+      <c r="C35" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
       <c r="G35" s="17"/>
       <c r="I35" s="11"/>
       <c r="J35" s="11"/>
@@ -4070,10 +4093,10 @@
     <row r="36" spans="1:68" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17"/>
       <c r="B36" s="17"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="17"/>
       <c r="H36" s="17"/>
       <c r="I36" s="11"/>
@@ -4140,12 +4163,12 @@
     <row r="37" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
-      <c r="C37" s="33" t="s">
+      <c r="C37" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="33"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
       <c r="G37" s="14"/>
       <c r="H37" s="14"/>
       <c r="I37" s="11"/>
@@ -4212,10 +4235,10 @@
     <row r="38" spans="1:68" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
       <c r="B38" s="17"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
       <c r="G38" s="14"/>
       <c r="H38" s="14"/>
       <c r="I38" s="11"/>
@@ -4282,10 +4305,10 @@
     <row r="39" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="13"/>
-      <c r="C39" s="35"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
       <c r="I39" s="2"/>
@@ -4352,10 +4375,10 @@
     <row r="40" spans="1:68" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
       <c r="I40" s="2"/>
@@ -4565,10 +4588,10 @@
       <c r="C43" s="15"/>
       <c r="D43" s="15"/>
       <c r="E43" s="15"/>
-      <c r="F43" s="37" t="s">
+      <c r="F43" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="G43" s="37"/>
+      <c r="G43" s="36"/>
       <c r="H43" s="15"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -4637,8 +4660,8 @@
       <c r="C44" s="15"/>
       <c r="D44" s="15"/>
       <c r="E44" s="15"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="36"/>
       <c r="H44" s="15"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -4707,8 +4730,8 @@
       <c r="C45" s="15"/>
       <c r="D45" s="15"/>
       <c r="E45" s="15"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="37"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="36"/>
       <c r="H45" s="16"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -4777,8 +4800,8 @@
       <c r="C46" s="15"/>
       <c r="D46" s="15"/>
       <c r="E46" s="15"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="37"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="36"/>
       <c r="H46" s="15"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -4847,8 +4870,8 @@
       <c r="C47" s="15"/>
       <c r="D47" s="15"/>
       <c r="E47" s="15"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="36"/>
       <c r="H47" s="15"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -4917,8 +4940,8 @@
       <c r="C48" s="15"/>
       <c r="D48" s="15"/>
       <c r="E48" s="15"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="37"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="36"/>
       <c r="H48" s="15"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -4987,8 +5010,8 @@
       <c r="C49" s="15"/>
       <c r="D49" s="15"/>
       <c r="E49" s="15"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="37"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="36"/>
       <c r="H49" s="15"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
@@ -5057,8 +5080,8 @@
       <c r="C50" s="15"/>
       <c r="D50" s="15"/>
       <c r="E50" s="15"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="37"/>
+      <c r="F50" s="36"/>
+      <c r="G50" s="36"/>
       <c r="H50" s="15"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -5127,8 +5150,8 @@
       <c r="C51" s="15"/>
       <c r="D51" s="15"/>
       <c r="E51" s="15"/>
-      <c r="F51" s="37"/>
-      <c r="G51" s="37"/>
+      <c r="F51" s="36"/>
+      <c r="G51" s="36"/>
       <c r="H51" s="15"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -5197,8 +5220,8 @@
       <c r="C52" s="15"/>
       <c r="D52" s="15"/>
       <c r="E52" s="15"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="37"/>
+      <c r="F52" s="36"/>
+      <c r="G52" s="36"/>
       <c r="H52" s="15"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -5267,8 +5290,8 @@
       <c r="C53" s="15"/>
       <c r="D53" s="15"/>
       <c r="E53" s="15"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="37"/>
+      <c r="F53" s="36"/>
+      <c r="G53" s="36"/>
       <c r="H53" s="15"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -5337,8 +5360,8 @@
       <c r="C54" s="15"/>
       <c r="D54" s="15"/>
       <c r="E54" s="15"/>
-      <c r="F54" s="37"/>
-      <c r="G54" s="37"/>
+      <c r="F54" s="36"/>
+      <c r="G54" s="36"/>
       <c r="H54" s="15"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -5477,8 +5500,8 @@
       <c r="C56" s="15"/>
       <c r="D56" s="15"/>
       <c r="E56" s="15"/>
-      <c r="F56" s="38"/>
-      <c r="G56" s="38"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="37"/>
       <c r="H56" s="15"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
@@ -5617,10 +5640,10 @@
       <c r="C58" s="15"/>
       <c r="D58" s="15"/>
       <c r="E58" s="15"/>
-      <c r="F58" s="41" t="s">
+      <c r="F58" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="G58" s="41"/>
+      <c r="G58" s="40"/>
       <c r="H58" s="15"/>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
@@ -5689,8 +5712,8 @@
       <c r="C59" s="15"/>
       <c r="D59" s="15"/>
       <c r="E59" s="15"/>
-      <c r="F59" s="41"/>
-      <c r="G59" s="41"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="40"/>
       <c r="H59" s="15"/>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
@@ -5759,8 +5782,8 @@
       <c r="C60" s="15"/>
       <c r="D60" s="15"/>
       <c r="E60" s="15"/>
-      <c r="F60" s="41"/>
-      <c r="G60" s="41"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="40"/>
       <c r="H60" s="15"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
@@ -5829,8 +5852,8 @@
       <c r="C61" s="15"/>
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
-      <c r="F61" s="41"/>
-      <c r="G61" s="41"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="40"/>
       <c r="H61" s="15"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
@@ -5899,8 +5922,8 @@
       <c r="C62" s="15"/>
       <c r="D62" s="15"/>
       <c r="E62" s="15"/>
-      <c r="F62" s="19"/>
-      <c r="G62" s="19"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
       <c r="H62" s="15"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
@@ -5969,8 +5992,8 @@
       <c r="C63" s="15"/>
       <c r="D63" s="15"/>
       <c r="E63" s="15"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="19"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
       <c r="H63" s="15"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
@@ -6039,12 +6062,12 @@
       <c r="C64" s="15"/>
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
-      <c r="F64" s="19"/>
-      <c r="G64" s="32" t="s">
+      <c r="F64" s="18"/>
+      <c r="G64" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="H64" s="32"/>
-      <c r="I64" s="32"/>
+      <c r="H64" s="31"/>
+      <c r="I64" s="31"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
@@ -6111,8 +6134,8 @@
       <c r="C65" s="15"/>
       <c r="D65" s="15"/>
       <c r="E65" s="15"/>
-      <c r="F65" s="18"/>
-      <c r="G65" s="20" t="s">
+      <c r="F65" s="15"/>
+      <c r="G65" s="19" t="s">
         <v>21</v>
       </c>
       <c r="H65" s="15"/>
@@ -16114,10 +16137,10 @@
     <mergeCell ref="F58:G61"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C37:F38" r:id="rId1" display="Comece agora | Grátis"/>
+    <hyperlink ref="C37:F38" r:id="rId1" display="Comece agora | Grátis" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
+  <pageSetup scale="10" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
   <drawing r:id="rId3"/>
   <tableParts count="1">
     <tablePart r:id="rId4"/>

</xml_diff>